<commit_message>
Part B: load/store, jump, upper
</commit_message>
<xml_diff>
--- a/RV32I.xlsx
+++ b/RV32I.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\machine_structures_cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DB76F8-34F0-4019-9EF6-52DCF02D1B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9C0957-7C51-4B70-863B-1041E7F7CEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D46B3F95-1030-460F-B0D5-F13F18E594E3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>RegWEn</t>
   </si>
@@ -633,7 +633,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,13 +1139,13 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1811,15 +1811,15 @@
       </c>
       <c r="J17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0061</v>
+        <v>0041</v>
       </c>
       <c r="K17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0061</v>
+        <v>0041</v>
       </c>
       <c r="L17" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>0061</v>
+        <v>0041</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
@@ -1879,6 +1879,9 @@
       </c>
       <c r="M19" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>53</v>
@@ -2093,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="N24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
@@ -2585,7 +2588,7 @@
       </c>
       <c r="N35" t="str">
         <f t="shared" si="19"/>
-        <v>2049</v>
+        <v>2041</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" si="19"/>

</xml_diff>